<commit_message>
Added grocery database in csv and excel format
</commit_message>
<xml_diff>
--- a/Items.xlsx
+++ b/Items.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quirk\Desktop\Grocery_Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beckc\OneDrive\Desktop\Projects\COSC341Proj\Grocery_Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94467A60-B7F6-4416-B081-9C17CA9EFDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3936E7B9-5B07-4B21-B60E-6962141C9BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{32A55907-A9F5-4067-B68E-C018D99242B5}"/>
+    <workbookView xWindow="-1170" yWindow="3600" windowWidth="29100" windowHeight="14160" xr2:uid="{32A55907-A9F5-4067-B68E-C018D99242B5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Items" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="35">
   <si>
     <t>Brand Name</t>
   </si>
@@ -66,6 +66,81 @@
   </si>
   <si>
     <t>Walmart</t>
+  </si>
+  <si>
+    <t>GroceryVille</t>
+  </si>
+  <si>
+    <t>Scrooge</t>
+  </si>
+  <si>
+    <t>Tasteful</t>
+  </si>
+  <si>
+    <t>Tavern</t>
+  </si>
+  <si>
+    <t>Yummy</t>
+  </si>
+  <si>
+    <t>Foodie</t>
+  </si>
+  <si>
+    <t>Peculiar</t>
+  </si>
+  <si>
+    <t>Safeway</t>
+  </si>
+  <si>
+    <t>Costco</t>
+  </si>
+  <si>
+    <t>Superstore</t>
+  </si>
+  <si>
+    <t>Save-On-Foods</t>
+  </si>
+  <si>
+    <t>Ketchup</t>
+  </si>
+  <si>
+    <t>Carrots</t>
+  </si>
+  <si>
+    <t>Potatoes</t>
+  </si>
+  <si>
+    <t>Baked Beans</t>
+  </si>
+  <si>
+    <t>Bread</t>
+  </si>
+  <si>
+    <t>Corn Flakes</t>
+  </si>
+  <si>
+    <t>Bacon</t>
+  </si>
+  <si>
+    <t>Brown Rice</t>
+  </si>
+  <si>
+    <t>Basmati Rice</t>
+  </si>
+  <si>
+    <t>Jasmine Rice</t>
+  </si>
+  <si>
+    <t>Instant Rice</t>
+  </si>
+  <si>
+    <t>Bananas</t>
+  </si>
+  <si>
+    <t>White Flour</t>
+  </si>
+  <si>
+    <t>Whole Wheat Flour</t>
   </si>
 </sst>
 </file>
@@ -107,7 +182,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -118,6 +197,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CD9E426D-D618-4548-AC6D-2D3E2B60D194}" name="Table1" displayName="Table1" ref="A1:G51" totalsRowShown="0">
+  <autoFilter ref="A1:G51" xr:uid="{CD9E426D-D618-4548-AC6D-2D3E2B60D194}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{A4BEFC16-2B1C-416E-BA44-C34A1BDDCA3D}" name="Brand Name"/>
+    <tableColumn id="2" xr3:uid="{C5174154-CD49-4A45-AD18-03A16F0CE26A}" name="Base Item"/>
+    <tableColumn id="3" xr3:uid="{762C28BF-F23C-49F7-B93A-F7D4A43753A6}" name="Price"/>
+    <tableColumn id="4" xr3:uid="{56629ED7-5A38-4DFB-A761-371B16419986}" name="Weight"/>
+    <tableColumn id="5" xr3:uid="{CBFC879F-E324-4CA3-9137-7E83CCB147C0}" name="Value"/>
+    <tableColumn id="6" xr3:uid="{0EBF1854-5F30-4768-A6D0-EDFC6DDFA46D}" name="Store"/>
+    <tableColumn id="7" xr3:uid="{FD35FE9A-5B30-47D5-B929-62997881D301}" name="File Name" dataDxfId="0">
+      <calculatedColumnFormula>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -417,23 +514,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE5F95F-1BD1-44F8-850A-4F4B3D138C3C}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,9 +554,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -474,10 +572,1242 @@
         <v>0.14635714285714285</v>
       </c>
       <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>foodie_white_rice.png</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="D3">
+        <v>12000</v>
+      </c>
+      <c r="E3">
+        <f>(C3/(D3/100))</f>
+        <v>0.16658333333333333</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>yummy_white_rice.png</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>10000</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E51" si="0">(C4/(D4/100))</f>
+        <v>0.15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>scrooge_white_rice.png</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>4.17</v>
+      </c>
+      <c r="D5">
+        <v>1000</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>groceryville_ketchup.png</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>2000</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>supercool_ketchup.png</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1000</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>foodie_ketchup.png</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>2.46</v>
+      </c>
+      <c r="D8">
+        <v>1000</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.246</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>foodie_carrots.png</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>2000</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>tasteful_carrots.png</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>10.33</v>
+      </c>
+      <c r="D10">
+        <v>4500</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.22955555555555557</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>tasteful_potatoes.png</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>1.51</v>
+      </c>
+      <c r="D11">
+        <v>400</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.3775</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>tasteful_baked_beans.png</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>800</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>yummy_baked_beans.png</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>1500</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>foodie_baked_beans.png</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>675</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>tasteful_bread.png</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>1200</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>scrooge_bread.png</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>800</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>tavern_bread.png</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>700</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="F17" t="s">
         <v>9</v>
+      </c>
+      <c r="G17" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>groceryville_bread.png</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>675</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>foodie_bread.png</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>2000</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>yummy_bread.png</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>5000</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>peculiar_bread.png</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
+        <v>6.38</v>
+      </c>
+      <c r="D21">
+        <v>675</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0.94518518518518513</v>
+      </c>
+      <c r="F21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>tavern_corn_flakes.png</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>1000</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>foodie_corn_flakes.png</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>700</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="F23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>yummy_corn_flakes.png</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>1200</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>scrooge_corn_flakes.png</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>400</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>tasteful_corn_flakes.png</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="D26">
+        <v>500</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>1.7100000000000002</v>
+      </c>
+      <c r="F26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>scrooge_bacon.png</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27">
+        <v>12</v>
+      </c>
+      <c r="D27">
+        <v>1000</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>supercool_bacon.png</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>35</v>
+      </c>
+      <c r="D28">
+        <v>5000</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="F28" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>tavern_bacon.png</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>700</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="F29" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>foodie_bacon.png</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>4.47</v>
+      </c>
+      <c r="D30">
+        <v>2000</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>0.22349999999999998</v>
+      </c>
+      <c r="F30" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>scrooge_brown_rice.png</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>4000</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="F31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>foodie_brown_rice.png</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32">
+        <v>2.75</v>
+      </c>
+      <c r="D32">
+        <v>1000</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="F32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>foodie_basmati_rice.png</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>7000</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="F33" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>tavern_basmati_rice.png</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34">
+        <v>30</v>
+      </c>
+      <c r="D34">
+        <v>15000</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>tavern_jasmine_rice.png</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>2000</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>foodie_jasmine_rice.png</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36">
+        <v>2.12</v>
+      </c>
+      <c r="D36">
+        <v>1000</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>0.21200000000000002</v>
+      </c>
+      <c r="F36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>tasteful_jasmine_rice.png</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37">
+        <v>11</v>
+      </c>
+      <c r="D37">
+        <v>5000</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>0.22</v>
+      </c>
+      <c r="F37" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>groceryville_jasmine_rice.png</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>500</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>supercool_jasmine_rice.png</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39">
+        <v>50</v>
+      </c>
+      <c r="D39">
+        <v>20000</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="F39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>tasteful_instant_rice.png</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40">
+        <v>25</v>
+      </c>
+      <c r="D40">
+        <v>12000</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="F40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>foodie_instant_rice.png</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41">
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>250</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+      <c r="F41" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>tavern_instant_rice.png</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>200</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>18</v>
+      </c>
+      <c r="G42" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>yummy_instant_rice.png</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43">
+        <v>12</v>
+      </c>
+      <c r="D43">
+        <v>1000</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>supercool_instant_rice.png</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44">
+        <v>1.63</v>
+      </c>
+      <c r="D44">
+        <v>1000</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>0.16299999999999998</v>
+      </c>
+      <c r="F44" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>tavern_bananas.png</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45">
+        <v>20</v>
+      </c>
+      <c r="D45">
+        <v>20000</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>supercool_bananas.png</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D46">
+        <v>2500</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>0.18600000000000003</v>
+      </c>
+      <c r="F46" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>tavern_white_flour.png</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47">
+        <v>30</v>
+      </c>
+      <c r="D47">
+        <v>30000</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>scrooge_white_flour.png</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48">
+        <v>7</v>
+      </c>
+      <c r="D48">
+        <v>2500</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F48" t="s">
+        <v>9</v>
+      </c>
+      <c r="G48" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>tavern_whole_wheat_flour.png</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49">
+        <v>20</v>
+      </c>
+      <c r="D49">
+        <v>6000</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F49" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>groceryville_whole_wheat_flour.png</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50">
+        <v>10</v>
+      </c>
+      <c r="D50">
+        <v>2000</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>19</v>
+      </c>
+      <c r="G50" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>peculiar_whole_wheat_flour.png</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51">
+        <v>14</v>
+      </c>
+      <c r="D51">
+        <v>3000</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="F51" t="s">
+        <v>19</v>
+      </c>
+      <c r="G51" t="str">
+        <f>LOWER(SUBSTITUTE(CONCATENATE(Table1[[#This Row],[Brand Name]]," ",Table1[[#This Row],[Base Item]],".png")," ","_"))</f>
+        <v>supercool_whole_wheat_flour.png</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>